<commit_message>
Modification de la documentation
</commit_message>
<xml_diff>
--- a/Documentations/Journal de travail.xlsx
+++ b/Documentations/Journal de travail.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\PréTPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PreTPI23\Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546B6EC7-E31E-4809-B536-95792F478D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D9EBA4-6AD3-483B-B017-63CC2865B149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
   <si>
     <t>Jour</t>
   </si>
@@ -105,13 +105,49 @@
     <t>Créer un MCD, MLD et des maquettes</t>
   </si>
   <si>
-    <t>0,15</t>
-  </si>
-  <si>
     <t>Modéliser une base de donnée</t>
   </si>
   <si>
     <t>Créer une connection à la base de donne avec php</t>
+  </si>
+  <si>
+    <t>0,30</t>
+  </si>
+  <si>
+    <t>Discution avec le maître de projet</t>
+  </si>
+  <si>
+    <t>1,15</t>
+  </si>
+  <si>
+    <t>Commencer le front-end de la page d'accueil</t>
+  </si>
+  <si>
+    <t>2,25</t>
+  </si>
+  <si>
+    <t>0,25</t>
+  </si>
+  <si>
+    <t>Remodéliser la base de donnée</t>
+  </si>
+  <si>
+    <t>1,00</t>
+  </si>
+  <si>
+    <t>Création et modification des backlogs</t>
+  </si>
+  <si>
+    <t>Compléter les infomations du IceScrum</t>
+  </si>
+  <si>
+    <t>Mettre à jour le MCD et MLD</t>
+  </si>
+  <si>
+    <t>Parfaire le rapport de projet</t>
+  </si>
+  <si>
+    <t>Modifier les maquettes</t>
   </si>
 </sst>
 </file>
@@ -182,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -219,7 +255,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,8 +594,8 @@
       <c r="B3" s="7">
         <v>1</v>
       </c>
-      <c r="C3" s="8">
-        <v>1</v>
+      <c r="C3" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>9</v>
@@ -722,13 +757,13 @@
         <v>2</v>
       </c>
       <c r="C12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>23</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>24</v>
       </c>
       <c r="F12" s="5"/>
     </row>
@@ -746,12 +781,153 @@
         <v>12</v>
       </c>
       <c r="E13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>44977</v>
+      </c>
+      <c r="B14" s="7">
+        <v>3</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="11"/>
+      <c r="D14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>44977</v>
+      </c>
+      <c r="B15" s="7">
+        <v>3</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>44977</v>
+      </c>
+      <c r="B16" s="7">
+        <v>3</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>45006</v>
+      </c>
+      <c r="B17" s="7">
+        <v>3</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>45008</v>
+      </c>
+      <c r="B18" s="7">
+        <v>3</v>
+      </c>
+      <c r="C18" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>45009</v>
+      </c>
+      <c r="B19" s="7">
+        <v>3</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>45009</v>
+      </c>
+      <c r="B20" s="7">
+        <v>3</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>45009</v>
+      </c>
+      <c r="B21" s="7">
+        <v>3</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Afficher les données de la base de données
</commit_message>
<xml_diff>
--- a/Documentations/Journal de travail.xlsx
+++ b/Documentations/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PreTPI23\Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44CFE12-95AD-44BC-B3F2-F44ED74BF914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964C10A3-7302-4898-9D41-1C6C54EE4285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="50">
   <si>
     <t>Jour</t>
   </si>
@@ -172,6 +172,18 @@
   </si>
   <si>
     <t>Modifier La base de données et retranscrire sur swisscenter</t>
+  </si>
+  <si>
+    <t>Afficher les valeurs de la base de données sur la page d'accueil et modifier le front-end</t>
+  </si>
+  <si>
+    <t>Créer un formulaire et afficher les nouvelles données</t>
+  </si>
+  <si>
+    <t>Créer un formulaire et afficher les nouvelles données, modifier le fichier php de connection</t>
+  </si>
+  <si>
+    <t>Finir le formulaire et mettre à jour les données sur swisscenter</t>
   </si>
 </sst>
 </file>
@@ -559,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,6 +1073,96 @@
       </c>
       <c r="F27" s="5"/>
     </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>44991</v>
+      </c>
+      <c r="B28" s="7">
+        <v>5</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>44991</v>
+      </c>
+      <c r="B29" s="7">
+        <v>5</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>44992</v>
+      </c>
+      <c r="B30" s="7">
+        <v>6</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>44994</v>
+      </c>
+      <c r="B31" s="7">
+        <v>7</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>44995</v>
+      </c>
+      <c r="B32" s="7">
+        <v>8</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F32" s="5"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>